<commit_message>
post draft commit with updates to the report, and some figures
</commit_message>
<xml_diff>
--- a/tables/inla models.xlsx
+++ b/tables/inla models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/NuWCRU/Analysis/NuWCRU/bim_2020/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C4ECBE8-9F3E-8445-9072-D9520406781E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1362E21-E820-184E-9617-41A9FF55BA31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43680" yWindow="2720" windowWidth="26440" windowHeight="15440" xr2:uid="{ED9CC9B4-3841-C84B-84B5-C3A434917F61}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Model</t>
   </si>
@@ -39,6 +39,9 @@
     <t>WAIC</t>
   </si>
   <si>
+    <t>fixed + spatial/time</t>
+  </si>
+  <si>
     <t>fixed + spatial/time/ar1</t>
   </si>
   <si>
@@ -46,6 +49,9 @@
   </si>
   <si>
     <t>fixed + spatial/time/iid</t>
+  </si>
+  <si>
+    <t>rlha</t>
   </si>
 </sst>
 </file>
@@ -403,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5883FEA-D396-484C-A5C5-7AB447F37F13}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -415,17 +421,17 @@
     <col min="4" max="4" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2"/>
       <c r="D1" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -453,7 +459,7 @@
         <v>217.78</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -466,33 +472,37 @@
       <c r="E4" s="1">
         <v>189.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <f>E3-E5</f>
+        <v>30.039999999999992</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>418.22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1">
-        <v>188.01</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>187.74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>418.71</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1">
-        <v>187.74</v>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <f>B6-B3</f>
+        <v>13.259999999999991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>